<commit_message>
Differential Horizontal Deflection Mixing Added.
Also, Dimensions spreadsheet adjusted.
</commit_message>
<xml_diff>
--- a/TODatabase/MachUp F-16 Dimensions.xlsx
+++ b/TODatabase/MachUp F-16 Dimensions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Christian\Documents\GitHub\F-16-Aero-Database\TODatabase\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50F5FF6C-1A77-48E4-917A-7C09AAC9F546}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{859ABCDF-8BD4-4508-9E66-E0CC40625C6B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20475" yWindow="1440" windowWidth="14400" windowHeight="11745" activeTab="3" xr2:uid="{3E8F2039-709E-449F-8242-523A09CEFF71}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{3E8F2039-709E-449F-8242-523A09CEFF71}"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="2" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="71">
   <si>
     <t>Fox</t>
   </si>
@@ -238,6 +238,18 @@
   </si>
   <si>
     <t>NACA 0004</t>
+  </si>
+  <si>
+    <t>Differential Deflection Limits, deg</t>
+  </si>
+  <si>
+    <t>Nguyen</t>
+  </si>
+  <si>
+    <t>Aileron Deflection Limits, deg</t>
+  </si>
+  <si>
+    <t>Differential Mixing Coefficient</t>
   </si>
 </sst>
 </file>
@@ -665,7 +677,7 @@
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -754,7 +766,8 @@
         <v>10</v>
       </c>
       <c r="B6" s="5">
-        <v>26.94</v>
+        <f>B4/C4*C6</f>
+        <v>26.941600000000005</v>
       </c>
       <c r="C6" s="5">
         <v>5.95</v>
@@ -798,7 +811,7 @@
   <dimension ref="A1:F38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A16" sqref="A16:A17"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -860,7 +873,7 @@
       </c>
       <c r="B4" s="12">
         <f>General!B6-'Main Wing'!B3</f>
-        <v>4.8659999999999997</v>
+        <v>4.867600000000003</v>
       </c>
       <c r="C4" s="14" t="s">
         <v>13</v>
@@ -1276,8 +1289,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA379603-7BA0-4D9A-95EF-34A9C14C4734}">
   <dimension ref="A1:F42"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A38" sqref="A38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1339,7 +1352,7 @@
       </c>
       <c r="B4" s="12">
         <f>General!B6-'Horizontal Tail'!B3</f>
-        <v>-12.940360000000002</v>
+        <v>-12.938759999999998</v>
       </c>
       <c r="C4" s="14" t="s">
         <v>13</v>
@@ -1795,12 +1808,38 @@
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A35" s="10"/>
-      <c r="C35" s="14"/>
+      <c r="A35" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="B35" s="12">
+        <v>5.375</v>
+      </c>
+      <c r="C35" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="D35" s="5" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A36" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="B36" s="12">
+        <v>21.5</v>
+      </c>
+      <c r="D36" s="5" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="37" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="3"/>
-      <c r="B37" s="12"/>
+      <c r="A37" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="B37" s="12">
+        <f>B35/B36</f>
+        <v>0.25</v>
+      </c>
       <c r="E37"/>
       <c r="F37"/>
     </row>
@@ -1844,8 +1883,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A5CE82D-4DDD-45B9-B0D1-292FAA56D14E}">
   <dimension ref="A1:F42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1907,7 +1946,7 @@
       </c>
       <c r="B4" s="12">
         <f>General!B6-'Vertical Tail'!B3</f>
-        <v>-11.128686328443354</v>
+        <v>-11.127086328443351</v>
       </c>
       <c r="C4" s="14" t="s">
         <v>13</v>
@@ -1958,7 +1997,7 @@
         <v>13</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>27</v>
+        <v>14</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -2076,7 +2115,7 @@
         <v>1</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>14</v>
+        <v>27</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
@@ -2164,7 +2203,7 @@
         <v>2.34</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>14</v>
+        <v>27</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
@@ -2209,7 +2248,7 @@
         <v>2.02</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>14</v>
+        <v>27</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
@@ -2224,7 +2263,7 @@
         <v>0.65</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>14</v>
+        <v>27</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
@@ -2239,7 +2278,7 @@
         <v>1.17</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>14</v>
+        <v>27</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
@@ -2254,7 +2293,7 @@
         <v>0.35</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>14</v>
+        <v>27</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>